<commit_message>
Aulas 4 e 5
</commit_message>
<xml_diff>
--- a/Frequencia/MAF105_Noite.xlsx
+++ b/Frequencia/MAF105_Noite.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="109">
   <si>
     <t>Nome do Aluno</t>
   </si>
@@ -488,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -508,9 +508,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -541,11 +538,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
@@ -557,125 +563,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -724,7 +611,35 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -753,41 +668,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1070,18 +950,22 @@
   <dimension ref="A1:AR50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM45" sqref="AM45"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="77" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="39" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="39" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="9.140625" style="1"/>
@@ -1093,39 +977,39 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11">
+      <c r="D1" s="10">
         <v>43319</v>
       </c>
-      <c r="E1" s="11">
+      <c r="E1" s="10">
         <v>43321</v>
       </c>
-      <c r="F1" s="11">
+      <c r="F1" s="10">
         <f t="shared" ref="F1:J1" si="0">D1+7</f>
         <v>43326</v>
       </c>
-      <c r="G1" s="11">
+      <c r="G1" s="10">
         <f t="shared" si="0"/>
         <v>43328</v>
       </c>
-      <c r="H1" s="11">
+      <c r="H1" s="10">
         <f t="shared" si="0"/>
         <v>43333</v>
       </c>
-      <c r="I1" s="12">
+      <c r="I1" s="11">
         <f t="shared" si="0"/>
         <v>43335</v>
       </c>
-      <c r="J1" s="11">
+      <c r="J1" s="10">
         <f t="shared" si="0"/>
         <v>43340</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="19">
         <f t="shared" ref="K1:AL1" si="1">I1+7</f>
         <v>43342</v>
       </c>
@@ -1133,7 +1017,7 @@
         <f t="shared" si="1"/>
         <v>43347</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="19">
         <f t="shared" si="1"/>
         <v>43349</v>
       </c>
@@ -1246,43 +1130,45 @@
       <c r="AO1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="9" t="s">
+      <c r="AQ1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="AR1" s="9"/>
+      <c r="AR1" s="21"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="D2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="20"/>
+      <c r="L2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="20"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
@@ -1311,7 +1197,7 @@
       <c r="AM2" s="6"/>
       <c r="AN2" s="6">
         <f>2*COUNTIF(D2:AM2,"="&amp;$AQ$2)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AO2" s="6">
         <f>2*COUNTIF(D2:AM2,"="&amp;$AR$2)</f>
@@ -1328,34 +1214,36 @@
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="D3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="14"/>
+      <c r="J3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="20"/>
+      <c r="L3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="20"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
@@ -1384,7 +1272,7 @@
       <c r="AM3" s="6"/>
       <c r="AN3" s="6">
         <f t="shared" ref="AN3:AN50" si="2">2*COUNTIF(D3:AM3,"="&amp;$AQ$2)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AO3" s="6">
         <f t="shared" ref="AO3:AO50" si="3">2*COUNTIF(D3:AM3,"="&amp;$AR$2)</f>
@@ -1395,34 +1283,36 @@
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="D4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="20"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
@@ -1451,7 +1341,7 @@
       <c r="AM4" s="6"/>
       <c r="AN4" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO4" s="6">
         <f t="shared" si="3"/>
@@ -1462,34 +1352,36 @@
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="D5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="20"/>
+      <c r="L5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="20"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
@@ -1518,7 +1410,7 @@
       <c r="AM5" s="6"/>
       <c r="AN5" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO5" s="6">
         <f t="shared" si="3"/>
@@ -1529,34 +1421,36 @@
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="D6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="20"/>
+      <c r="L6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="20"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -1589,41 +1483,43 @@
       </c>
       <c r="AO6" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <v>2004</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>145</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="D7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="20"/>
+      <c r="L7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="20"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
@@ -1652,7 +1548,7 @@
       <c r="AM7" s="6"/>
       <c r="AN7" s="6">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AO7" s="6">
         <f t="shared" si="3"/>
@@ -1663,35 +1559,39 @@
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="D8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="20"/>
+      <c r="L8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="20"/>
+      <c r="N8" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
@@ -1719,45 +1619,47 @@
       <c r="AM8" s="6"/>
       <c r="AN8" s="6">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AO8" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="17">
         <v>2068</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="D9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="L9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="20"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -1786,45 +1688,47 @@
       <c r="AM9" s="6"/>
       <c r="AN9" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AO9" s="6">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="D10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="20"/>
+      <c r="L10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="20"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -1853,7 +1757,7 @@
       <c r="AM10" s="6"/>
       <c r="AN10" s="6">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AO10" s="6">
         <f t="shared" si="3"/>
@@ -1864,34 +1768,36 @@
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="D11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="20"/>
+      <c r="L11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="20"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
@@ -1920,7 +1826,7 @@
       <c r="AM11" s="6"/>
       <c r="AN11" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO11" s="6">
         <f t="shared" si="3"/>
@@ -1931,34 +1837,36 @@
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="D12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="20"/>
+      <c r="L12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="20"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
@@ -1987,7 +1895,7 @@
       <c r="AM12" s="6"/>
       <c r="AN12" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO12" s="6">
         <f t="shared" si="3"/>
@@ -1998,34 +1906,36 @@
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="D13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="20"/>
+      <c r="L13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="20"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
@@ -2054,7 +1964,7 @@
       <c r="AM13" s="6"/>
       <c r="AN13" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO13" s="6">
         <f t="shared" si="3"/>
@@ -2065,34 +1975,36 @@
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="D14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="20"/>
+      <c r="L14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="20"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
@@ -2121,7 +2033,7 @@
       <c r="AM14" s="6"/>
       <c r="AN14" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO14" s="6">
         <f t="shared" si="3"/>
@@ -2132,34 +2044,36 @@
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="D15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="20"/>
+      <c r="L15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="20"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
@@ -2188,7 +2102,7 @@
       <c r="AM15" s="6"/>
       <c r="AN15" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO15" s="6">
         <f t="shared" si="3"/>
@@ -2199,34 +2113,36 @@
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="D16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="20"/>
+      <c r="L16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="20"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
@@ -2255,7 +2171,7 @@
       <c r="AM16" s="6"/>
       <c r="AN16" s="6">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AO16" s="6">
         <f t="shared" si="3"/>
@@ -2266,34 +2182,36 @@
       <c r="A17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+      <c r="D17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="14"/>
+      <c r="J17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="20"/>
+      <c r="L17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="20"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
@@ -2322,7 +2240,7 @@
       <c r="AM17" s="6"/>
       <c r="AN17" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO17" s="6">
         <f t="shared" si="3"/>
@@ -2333,34 +2251,36 @@
       <c r="A18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="D18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="20"/>
+      <c r="L18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="20"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
@@ -2389,7 +2309,7 @@
       <c r="AM18" s="6"/>
       <c r="AN18" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO18" s="6">
         <f t="shared" si="3"/>
@@ -2400,34 +2320,36 @@
       <c r="A19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="D19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="14"/>
+      <c r="J19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="20"/>
+      <c r="L19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M19" s="20"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
@@ -2460,41 +2382,43 @@
       </c>
       <c r="AO19" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
+      <c r="D20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="14"/>
+      <c r="J20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" s="20"/>
+      <c r="L20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" s="20"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
@@ -2527,41 +2451,43 @@
       </c>
       <c r="AO20" s="6">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="D21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="14"/>
+      <c r="J21" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" s="20"/>
+      <c r="L21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="20"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
@@ -2594,41 +2520,43 @@
       </c>
       <c r="AO21" s="6">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="D22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="14"/>
+      <c r="J22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="20"/>
+      <c r="L22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22" s="20"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
@@ -2661,41 +2589,43 @@
       </c>
       <c r="AO22" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="D23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="14"/>
+      <c r="J23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="20"/>
+      <c r="L23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23" s="20"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
@@ -2724,7 +2654,7 @@
       <c r="AM23" s="6"/>
       <c r="AN23" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO23" s="6">
         <f t="shared" si="3"/>
@@ -2735,34 +2665,36 @@
       <c r="A24" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="D24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="14"/>
+      <c r="J24" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="20"/>
+      <c r="L24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" s="20"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
@@ -2795,41 +2727,43 @@
       </c>
       <c r="AO24" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="D25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="20"/>
+      <c r="L25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" s="20"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
@@ -2858,7 +2792,7 @@
       <c r="AM25" s="6"/>
       <c r="AN25" s="6">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AO25" s="6">
         <f t="shared" si="3"/>
@@ -2869,34 +2803,36 @@
       <c r="A26" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="15"/>
-      <c r="J26" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="D26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="14"/>
+      <c r="J26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="20"/>
+      <c r="L26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" s="20"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
@@ -2925,7 +2861,7 @@
       <c r="AM26" s="6"/>
       <c r="AN26" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO26" s="6">
         <f t="shared" si="3"/>
@@ -2936,34 +2872,36 @@
       <c r="A27" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+      <c r="D27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="14"/>
+      <c r="J27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" s="20"/>
+      <c r="L27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M27" s="20"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
@@ -2992,7 +2930,7 @@
       <c r="AM27" s="6"/>
       <c r="AN27" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO27" s="6">
         <f t="shared" si="3"/>
@@ -3003,34 +2941,36 @@
       <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I28" s="15"/>
-      <c r="J28" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
+      <c r="D28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I28" s="14"/>
+      <c r="J28" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K28" s="20"/>
+      <c r="L28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M28" s="20"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
@@ -3063,41 +3003,43 @@
       </c>
       <c r="AO28" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I29" s="15"/>
-      <c r="J29" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
+      <c r="D29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="14"/>
+      <c r="J29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="20"/>
+      <c r="L29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="20"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
@@ -3126,7 +3068,7 @@
       <c r="AM29" s="6"/>
       <c r="AN29" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO29" s="6">
         <f t="shared" si="3"/>
@@ -3137,34 +3079,36 @@
       <c r="A30" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
+      <c r="D30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="14"/>
+      <c r="J30" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" s="20"/>
+      <c r="L30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M30" s="20"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
@@ -3197,41 +3141,43 @@
       </c>
       <c r="AO30" s="6">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I31" s="15"/>
-      <c r="J31" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
+      <c r="D31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="14"/>
+      <c r="J31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="20"/>
+      <c r="L31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="20"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
@@ -3260,7 +3206,7 @@
       <c r="AM31" s="6"/>
       <c r="AN31" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO31" s="6">
         <f t="shared" si="3"/>
@@ -3271,34 +3217,36 @@
       <c r="A32" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I32" s="15"/>
-      <c r="J32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
+      <c r="D32" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="14"/>
+      <c r="J32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="20"/>
+      <c r="L32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="20"/>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
@@ -3327,7 +3275,7 @@
       <c r="AM32" s="6"/>
       <c r="AN32" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO32" s="6">
         <f t="shared" si="3"/>
@@ -3338,34 +3286,36 @@
       <c r="A33" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I33" s="15"/>
-      <c r="J33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
+      <c r="D33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="14"/>
+      <c r="J33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="20"/>
+      <c r="L33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" s="20"/>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
@@ -3394,7 +3344,7 @@
       <c r="AM33" s="6"/>
       <c r="AN33" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO33" s="6">
         <f t="shared" si="3"/>
@@ -3405,34 +3355,36 @@
       <c r="A34" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I34" s="15"/>
-      <c r="J34" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
+      <c r="D34" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="14"/>
+      <c r="J34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="20"/>
+      <c r="L34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M34" s="20"/>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
@@ -3465,41 +3417,43 @@
       </c>
       <c r="AO34" s="6">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I35" s="15"/>
-      <c r="J35" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
+      <c r="D35" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="14"/>
+      <c r="J35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="20"/>
+      <c r="L35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="20"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
@@ -3528,7 +3482,7 @@
       <c r="AM35" s="6"/>
       <c r="AN35" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO35" s="6">
         <f t="shared" si="3"/>
@@ -3539,34 +3493,36 @@
       <c r="A36" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I36" s="15"/>
-      <c r="J36" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
+      <c r="D36" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="14"/>
+      <c r="J36" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="20"/>
+      <c r="L36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" s="20"/>
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
@@ -3595,7 +3551,7 @@
       <c r="AM36" s="6"/>
       <c r="AN36" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO36" s="6">
         <f t="shared" si="3"/>
@@ -3606,34 +3562,36 @@
       <c r="A37" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I37" s="15"/>
-      <c r="J37" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
+      <c r="D37" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="14"/>
+      <c r="J37" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="20"/>
+      <c r="L37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="20"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
@@ -3662,7 +3620,7 @@
       <c r="AM37" s="6"/>
       <c r="AN37" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO37" s="6">
         <f t="shared" si="3"/>
@@ -3673,34 +3631,36 @@
       <c r="A38" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" s="15"/>
-      <c r="J38" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
+      <c r="D38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="14"/>
+      <c r="J38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" s="20"/>
+      <c r="L38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M38" s="20"/>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
@@ -3729,7 +3689,7 @@
       <c r="AM38" s="6"/>
       <c r="AN38" s="6">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AO38" s="6">
         <f t="shared" si="3"/>
@@ -3740,34 +3700,36 @@
       <c r="A39" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I39" s="15"/>
-      <c r="J39" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
+      <c r="D39" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="14"/>
+      <c r="J39" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="20"/>
+      <c r="L39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M39" s="20"/>
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
@@ -3796,7 +3758,7 @@
       <c r="AM39" s="6"/>
       <c r="AN39" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO39" s="6">
         <f t="shared" si="3"/>
@@ -3807,34 +3769,36 @@
       <c r="A40" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I40" s="15"/>
-      <c r="J40" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
+      <c r="D40" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="14"/>
+      <c r="J40" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" s="20"/>
+      <c r="L40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M40" s="20"/>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
@@ -3863,7 +3827,7 @@
       <c r="AM40" s="6"/>
       <c r="AN40" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO40" s="6">
         <f t="shared" si="3"/>
@@ -3874,34 +3838,36 @@
       <c r="A41" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" s="15"/>
-      <c r="J41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
+      <c r="D41" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="14"/>
+      <c r="J41" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" s="20"/>
+      <c r="L41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M41" s="20"/>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
@@ -3930,7 +3896,7 @@
       <c r="AM41" s="6"/>
       <c r="AN41" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO41" s="6">
         <f t="shared" si="3"/>
@@ -3941,34 +3907,36 @@
       <c r="A42" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I42" s="15"/>
-      <c r="J42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
+      <c r="D42" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="14"/>
+      <c r="J42" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K42" s="20"/>
+      <c r="L42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M42" s="20"/>
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
@@ -3997,7 +3965,7 @@
       <c r="AM42" s="6"/>
       <c r="AN42" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO42" s="6">
         <f t="shared" si="3"/>
@@ -4008,34 +3976,36 @@
       <c r="A43" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I43" s="15"/>
-      <c r="J43" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
+      <c r="D43" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="14"/>
+      <c r="J43" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="20"/>
+      <c r="L43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M43" s="20"/>
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
@@ -4064,7 +4034,7 @@
       <c r="AM43" s="6"/>
       <c r="AN43" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO43" s="6">
         <f t="shared" si="3"/>
@@ -4075,34 +4045,36 @@
       <c r="A44" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I44" s="15"/>
-      <c r="J44" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
+      <c r="D44" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="14"/>
+      <c r="J44" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K44" s="20"/>
+      <c r="L44" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M44" s="20"/>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
@@ -4131,7 +4103,7 @@
       <c r="AM44" s="6"/>
       <c r="AN44" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO44" s="6">
         <f t="shared" si="3"/>
@@ -4142,34 +4114,36 @@
       <c r="A45" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B45" s="17">
         <v>3056</v>
       </c>
-      <c r="C45" s="13">
+      <c r="C45" s="12">
         <v>107</v>
       </c>
-      <c r="D45" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I45" s="15"/>
-      <c r="J45" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
+      <c r="D45" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="14"/>
+      <c r="J45" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K45" s="20"/>
+      <c r="L45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M45" s="20"/>
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
@@ -4198,7 +4172,7 @@
       <c r="AM45" s="6"/>
       <c r="AN45" s="6">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AO45" s="6">
         <f t="shared" si="3"/>
@@ -4209,34 +4183,36 @@
       <c r="A46" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H46" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I46" s="15"/>
-      <c r="J46" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-      <c r="M46" s="6"/>
+      <c r="D46" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="14"/>
+      <c r="J46" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K46" s="20"/>
+      <c r="L46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M46" s="20"/>
       <c r="N46" s="6"/>
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
@@ -4269,41 +4245,43 @@
       </c>
       <c r="AO46" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I47" s="15"/>
-      <c r="J47" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
+      <c r="D47" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="14"/>
+      <c r="J47" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47" s="20"/>
+      <c r="L47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M47" s="20"/>
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
@@ -4332,7 +4310,7 @@
       <c r="AM47" s="6"/>
       <c r="AN47" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO47" s="6">
         <f t="shared" si="3"/>
@@ -4343,34 +4321,36 @@
       <c r="A48" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="19" t="s">
+      <c r="B48" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I48" s="15"/>
-      <c r="J48" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
+      <c r="D48" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="14"/>
+      <c r="J48" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" s="20"/>
+      <c r="L48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M48" s="20"/>
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
@@ -4403,41 +4383,43 @@
       </c>
       <c r="AO48" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B49" s="19" t="s">
+      <c r="B49" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I49" s="15"/>
-      <c r="J49" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
-      <c r="M49" s="6"/>
+      <c r="D49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="14"/>
+      <c r="J49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K49" s="20"/>
+      <c r="L49" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M49" s="20"/>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
@@ -4466,7 +4448,7 @@
       <c r="AM49" s="6"/>
       <c r="AN49" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AO49" s="6">
         <f t="shared" si="3"/>
@@ -4477,34 +4459,36 @@
       <c r="A50" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D50" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I50" s="15"/>
-      <c r="J50" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
+      <c r="D50" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" s="14"/>
+      <c r="J50" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K50" s="20"/>
+      <c r="L50" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M50" s="20"/>
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
@@ -4533,7 +4517,7 @@
       <c r="AM50" s="6"/>
       <c r="AN50" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AO50" s="6">
         <f t="shared" si="3"/>
@@ -4552,52 +4536,52 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:AM50">
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="Ausente">
+    <cfRule type="containsText" dxfId="16" priority="15" operator="containsText" text="Ausente">
       <formula>NOT(ISERROR(SEARCH("Ausente",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="Presente">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="Presente">
       <formula>NOT(ISERROR(SEARCH("Presente",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:F5">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Presença">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Presença">
       <formula>NOT(ISERROR(SEARCH("Presença",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:E5">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Ausência">
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="Ausência">
       <formula>NOT(ISERROR(SEARCH("Ausência",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:J6 D8:J8 D46:J50 D10:J44">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Ausente">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="Ausente">
       <formula>NOT(ISERROR(SEARCH("Ausente",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Presente">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="Presente">
       <formula>NOT(ISERROR(SEARCH("Presente",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:J9">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Ausente">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Ausente">
       <formula>NOT(ISERROR(SEARCH("Ausente",D9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Presente">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Presente">
       <formula>NOT(ISERROR(SEARCH("Presente",D9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:J7">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Ausente">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Ausente">
       <formula>NOT(ISERROR(SEARCH("Ausente",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Presente">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Presente">
       <formula>NOT(ISERROR(SEARCH("Presente",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:J45">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Ausente">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Ausente">
       <formula>NOT(ISERROR(SEARCH("Ausente",D45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Presente">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Presente">
       <formula>NOT(ISERROR(SEARCH("Presente",D45)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>